<commit_message>
update refinance comparison to allow for manual input to outstanding
</commit_message>
<xml_diff>
--- a/assets/worksheets/RefinancingPaymentComparison.xlsx
+++ b/assets/worksheets/RefinancingPaymentComparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f86cf31dab8dac97/Documents/Work/Public Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="511" documentId="11_800E462303CA0CC5A985D5AC4394A92BBCEA1CB8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF0CC0E3-E1DE-42F6-8C46-0E1868BFC6CB}"/>
+  <xr:revisionPtr revIDLastSave="516" documentId="11_800E462303CA0CC5A985D5AC4394A92BBCEA1CB8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2D887B2B-9F89-4A22-B420-A7B62BB52C4E}"/>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="2130" windowWidth="14400" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6720" yWindow="2325" windowWidth="14400" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="3" r:id="rId1"/>
@@ -261,7 +261,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -419,6 +419,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -872,11 +876,11 @@
       </c>
       <c r="C4" s="39">
         <f ca="1">EOMONTH(TODAY()+60,-1)+1</f>
-        <v>43983</v>
+        <v>44013</v>
       </c>
       <c r="D4" s="39">
         <f ca="1">C4</f>
-        <v>43983</v>
+        <v>44013</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -886,7 +890,7 @@
       <c r="B5" s="40">
         <v>3275000</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="59">
         <f ca="1">B9</f>
         <v>3110000</v>
       </c>
@@ -1097,7 +1101,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C13:D13 D6:D7 B12" unlockedFormula="1"/>
+    <ignoredError sqref="C13:D13 D6:D7 B12 C5" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1171,7 +1175,7 @@
       </c>
       <c r="B5" s="28">
         <f ca="1">30-(TODAY()-DATE(2017,6,27))/365.25</f>
-        <v>27.160848733744011</v>
+        <v>27.138945927446954</v>
       </c>
       <c r="C5" s="4">
         <v>30</v>
@@ -1201,7 +1205,7 @@
       </c>
       <c r="B7" s="15">
         <f ca="1">PMT(B6/12,B5*12,-B4)</f>
-        <v>16112.865430393542</v>
+        <v>16119.785854290947</v>
       </c>
       <c r="C7" s="15">
         <f t="shared" ref="C7:D7" si="0">PMT(C6/12,C5*12,-C4)</f>
@@ -1219,11 +1223,11 @@
       <c r="B8" s="24"/>
       <c r="C8" s="16">
         <f ca="1">C7-$B$7</f>
-        <v>-2396.6439781655572</v>
+        <v>-2403.5644020629625</v>
       </c>
       <c r="D8" s="17">
         <f ca="1">D7-$B$7</f>
-        <v>-247.17831651908273</v>
+        <v>-254.098740416488</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1284,11 +1288,11 @@
       <c r="B13" s="21"/>
       <c r="C13" s="18">
         <f ca="1">C12/-C8</f>
-        <v>22.669199303262953</v>
+        <v>22.603929378122317</v>
       </c>
       <c r="D13" s="18">
         <f ca="1">D12/-D8</f>
-        <v>219.80083352418819</v>
+        <v>213.81451915483257</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1308,7 +1312,7 @@
       </c>
       <c r="B15" s="15">
         <f ca="1">CUMIPMT(B6/12,B5*12,B4,1,1+$B$14*12,0)*-1</f>
-        <v>636969.44902490114</v>
+        <v>636921.30475637666</v>
       </c>
       <c r="C15" s="15">
         <f>CUMIPMT(C6/12,C5*12,C4,1,$B$14*12,0)*-1</f>
@@ -1327,11 +1331,11 @@
       <c r="B16" s="27"/>
       <c r="C16" s="23">
         <f ca="1">$B$15-C15</f>
-        <v>141902.67168135638</v>
+        <v>141854.5274128319</v>
       </c>
       <c r="D16" s="23">
         <f ca="1">$B$15-D15</f>
-        <v>64320.879798790789</v>
+        <v>64272.735530266305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>